<commit_message>
ASLDRO-49: perfusion_rate is now correctly scaled from ml/100g/min input to ml/g/s, added docstring
</commit_message>
<xml_diff>
--- a/src/asldro/data/gkm_validation_calculations.xlsx
+++ b/src/asldro/data/gkm_validation_calculations.xlsx
@@ -5,40 +5,40 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5FFE8B-B4F0-4196-AF92-99F601402FBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E6BD5C-A31B-4833-B35F-64367411573E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PASL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="alpha">PASL!$B$9</definedName>
-    <definedName name="delta_m">PASL!$B$19</definedName>
-    <definedName name="delta_m_arrived">PASL!$B$18</definedName>
-    <definedName name="delta_m_arriving">PASL!$B$17</definedName>
-    <definedName name="delta_m_not_arrived">PASL!$B$17</definedName>
-    <definedName name="delta_m_not_arriving">PASL!$B$17</definedName>
+    <definedName name="delta_m">PASL!$B$20</definedName>
+    <definedName name="delta_m_arrived">PASL!$B$19</definedName>
+    <definedName name="delta_m_arriving">PASL!$B$18</definedName>
+    <definedName name="delta_m_not_arrived">PASL!$B$18</definedName>
+    <definedName name="delta_m_not_arriving">PASL!$B$18</definedName>
     <definedName name="delta_t">PASL!$B$6</definedName>
     <definedName name="f">PASL!$B$5</definedName>
-    <definedName name="k">PASL!$B$14</definedName>
+    <definedName name="k">PASL!$B$15</definedName>
     <definedName name="label_duration">PASL!$B$8</definedName>
     <definedName name="label_efficiency">PASL!$B$9</definedName>
     <definedName name="lambda">PASL!$B$10</definedName>
     <definedName name="lambda_blood_brain">PASL!$B$10</definedName>
     <definedName name="m0">PASL!$B$7</definedName>
     <definedName name="perfusion_rate">PASL!$B$5</definedName>
-    <definedName name="q_pasl_arrived">PASL!$B$16</definedName>
-    <definedName name="q_pasl_arriving">PASL!$B$15</definedName>
+    <definedName name="q_pasl_arrived">PASL!$B$17</definedName>
+    <definedName name="q_pasl_arriving">PASL!$B$16</definedName>
     <definedName name="signal_time">PASL!$B$12</definedName>
     <definedName name="t">PASL!$B$12</definedName>
     <definedName name="t1_arterial_blood">PASL!$B$11</definedName>
-    <definedName name="t1_prime">PASL!$B$13</definedName>
+    <definedName name="t1_prime">PASL!$B$14</definedName>
     <definedName name="t1b">PASL!$B$11</definedName>
-    <definedName name="t1p">PASL!$B$13</definedName>
+    <definedName name="t1p">PASL!$B$14</definedName>
     <definedName name="tau">PASL!$B$8</definedName>
     <definedName name="transit_time">PASL!$B$6</definedName>
   </definedNames>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>General Kinetic Model Valitation Calculator</t>
   </si>
@@ -118,13 +118,17 @@
   <si>
     <t>delta_m_arriving</t>
   </si>
+  <si>
+    <t>f</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="177" formatCode="0.00000000000000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -181,14 +185,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,9 +346,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PASL!$B$19:$AA$19</c:f>
+              <c:f>PASL!$B$20:$AA$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000000000000E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -363,64 +369,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13009645818687179</c:v>
+                  <c:v>1.3738151855842728E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23157648392212382</c:v>
+                  <c:v>2.5797266811167139E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30947841216999944</c:v>
+                  <c:v>3.6331253852959419E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36800865332861948</c:v>
+                  <c:v>4.5481481153741609E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.41067603525134655</c:v>
+                  <c:v>5.3377734080001958E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44040462813087888</c:v>
+                  <c:v>6.0139102942783386E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.45962848800173517</c:v>
+                  <c:v>6.5874805499984432E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47037120664903925</c:v>
+                  <c:v>7.0684948869971995E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.47431269510044394</c:v>
+                  <c:v>7.4661235190256591E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.47284524069961731</c:v>
+                  <c:v>7.7887615051586822E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.39748493625481746</c:v>
+                  <c:v>7.3087389667719441E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.33413527503360196</c:v>
+                  <c:v>6.85830028933751E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28088204567885094</c:v>
+                  <c:v>6.4356222150729649E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.23611611667400922</c:v>
+                  <c:v>6.0389938538461755E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.19848481386011235</c:v>
+                  <c:v>5.6668097579401491E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.16685104722214014</c:v>
+                  <c:v>5.3175634236212067E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14025895189515777</c:v>
+                  <c:v>4.9898411932064613E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.11790500517828191</c:v>
+                  <c:v>4.6823165329478002E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.9113746810841549E-2</c:v>
+                  <c:v>4.3937446635707329E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.3317368860037988E-2</c:v>
+                  <c:v>4.1229575217339321E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -526,7 +532,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000000000000E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1181,13 +1187,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>198664</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>59871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>198664</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>27214</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1479,148 +1485,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AB20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:AA19"/>
+      <selection activeCell="B20" sqref="B20:AA20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.765625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="H5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="I5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="J5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="K5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="L5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="M5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="N5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="O5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="P5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="R5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="S5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="T5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="U5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="V5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="W5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="X5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="Y5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="Z5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="AA5" s="5">
-        <f>1</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="AB5" s="5"/>
     </row>
-    <row r="6" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1704,7 +1686,7 @@
       </c>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1788,7 +1770,7 @@
       </c>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1872,7 +1854,7 @@
       </c>
       <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1956,7 +1938,7 @@
       </c>
       <c r="AB9" s="5"/>
     </row>
-    <row r="10" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2040,7 +2022,7 @@
       </c>
       <c r="AB10" s="5"/>
     </row>
-    <row r="11" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2124,7 +2106,7 @@
       </c>
       <c r="AB11" s="5"/>
     </row>
-    <row r="12" spans="1:28" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:28" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2208,773 +2190,883 @@
       </c>
       <c r="AB12" s="5"/>
     </row>
-    <row r="13" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:28" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="C13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="H13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="I13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="K13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="L13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="M13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="N13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="O13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="P13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="Q13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="R13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="S13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="T13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="U13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="V13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="W13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="X13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="Y13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="Z13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="AA13" s="7">
+        <f>f/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6">
-        <f>1/(1/B11+B5/B10)</f>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="C13" s="6">
-        <f t="shared" ref="C13:U13" si="0">1/(1/C11+C5/C10)</f>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="B14" s="6">
+        <f>1/(1/B11+B13/B10)</f>
+        <v>1.572052401746725</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" ref="C14:AA14" si="0">1/(1/C11+C13/C10)</f>
+        <v>1.572052401746725</v>
+      </c>
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="E13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="F13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="G13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="H13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="I13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="J13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="J14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="K13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="K14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="L13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="M13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="N13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="N14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="O13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="O14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="P13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="P14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="Q13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="Q14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="R13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="R14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="S13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="S14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="T13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="U13" s="6">
+        <v>1.572052401746725</v>
+      </c>
+      <c r="U14" s="6">
         <f t="shared" si="0"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="V13" s="6">
-        <f t="shared" ref="V13:AB13" si="1">1/(1/V11+V5/V10)</f>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="W13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="X13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="Y13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="Z13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="AA13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="AB13" s="6"/>
-    </row>
-    <row r="14" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="6">
-        <f>(1/B11-1/B13)</f>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="C14" s="6">
-        <f t="shared" ref="C14:U14" si="2">(1/C11-1/C13)</f>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="D14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="E14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="F14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="H14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="I14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="J14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="K14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="L14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="N14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="O14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="P14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="Q14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="R14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="S14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="T14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
-      </c>
-      <c r="U14" s="6">
-        <f t="shared" si="2"/>
-        <v>-1.1111111111111112</v>
+        <v>1.572052401746725</v>
       </c>
       <c r="V14" s="6">
-        <f t="shared" ref="V14" si="3">(1/V11-1/V13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="W14" s="6">
-        <f t="shared" ref="W14" si="4">(1/W11-1/W13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="X14" s="6">
-        <f t="shared" ref="X14" si="5">(1/X11-1/X13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="Y14" s="6">
-        <f t="shared" ref="Y14" si="6">(1/Y11-1/Y13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="Z14" s="6">
-        <f t="shared" ref="Z14" si="7">(1/Z11-1/Z13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="AA14" s="6">
-        <f t="shared" ref="AA14" si="8">(1/AA11-1/AA13)</f>
-        <v>-1.1111111111111112</v>
+        <f t="shared" si="0"/>
+        <v>1.572052401746725</v>
       </c>
       <c r="AB14" s="6"/>
     </row>
-    <row r="15" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B15" s="6">
-        <f>EXP(B14 * B12) * (EXP(- B14 * B6) - EXP(- B14 * B12)) / (B14 * (B12 - B6))</f>
-        <v>1.337236197540224</v>
+        <f>(1/B11-1/B14)</f>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" ref="C15:U15" si="9">EXP(C14 * C12) * (EXP(- C14 * C6) - EXP(- C14 * C12)) / (C14 * (C12 - C6))</f>
-        <v>1.2591528696152565</v>
+        <f t="shared" ref="C15:AA15" si="1">(1/C11-1/C14)</f>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="9"/>
-        <v>1.186837275258269</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="9"/>
-        <v>1.1198199105075699</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="9"/>
-        <v>1.0576716186767723</v>
-      </c>
-      <c r="G15" s="6" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.94644614867067145</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.89668168687436411</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.8504060682786323</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.80734412603260208</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.76724384267262102</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.72987432145111186</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.69502394052523708</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.66249867317941424</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.63212055882855778</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="Q15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.60372631097288498</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="R15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.57716604956445761</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="S15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.55230214641320496</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="T15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.52900817331759231</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="U15" s="6">
-        <f t="shared" si="9"/>
-        <v>0.50716794356287065</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="V15" s="6">
-        <f t="shared" ref="V15" si="10">EXP(V14 * V12) * (EXP(- V14 * V6) - EXP(- V14 * V12)) / (V14 * (V12 - V6))</f>
-        <v>0.48667463829746282</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="W15" s="6">
-        <f t="shared" ref="W15" si="11">EXP(W14 * W12) * (EXP(- W14 * W6) - EXP(- W14 * W12)) / (W14 * (W12 - W6))</f>
-        <v>0.4674300100840878</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="X15" s="6">
-        <f t="shared" ref="X15" si="12">EXP(X14 * X12) * (EXP(- X14 * X6) - EXP(- X14 * X12)) / (X14 * (X12 - X6))</f>
-        <v>0.44934365663444331</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="Y15" s="6">
-        <f t="shared" ref="Y15" si="13">EXP(Y14 * Y12) * (EXP(- Y14 * Y6) - EXP(- Y14 * Y12)) / (Y14 * (Y12 - Y6))</f>
-        <v>0.43233235838169365</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="Z15" s="6">
-        <f t="shared" ref="Z15" si="14">EXP(Z14 * Z12) * (EXP(- Z14 * Z6) - EXP(- Z14 * Z12)) / (Z14 * (Z12 - Z6))</f>
-        <v>0.41631947412994902</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="AA15" s="6">
-        <f t="shared" ref="AA15" si="15">EXP(AA14 * AA12) * (EXP(- AA14 * AA6) - EXP(- AA14 * AA12)) / (AA14 * (AA12 - AA6))</f>
-        <v>0.40123438955014679</v>
+        <f t="shared" si="1"/>
+        <v>-1.1111111111111072E-2</v>
       </c>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="6">
-        <f>EXP(B14 * B12) * (EXP(-B14 * B6) - EXP(-B14 * (B8 + B6))) / (B14 * B8)</f>
-        <v>3.1964229466529148</v>
+        <f>EXP(B15 * B12) * (EXP(- B15 * B6) - EXP(- B15 * B12)) / (B15 * (B12 - B6))</f>
+        <v>1.0027829289631542</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" ref="C16:U16" si="16">EXP(C14 * C12) * (EXP(-C14 * C6) - EXP(-C14 * (C8 + C6))) / (C14 * C8)</f>
-        <v>2.8602849258326688</v>
+        <f t="shared" ref="C16:AA16" si="2">EXP(C15 * C12) * (EXP(- C15 * C6) - EXP(- C15 * C12)) / (C15 * (C12 - C6))</f>
+        <v>1.0022255180645383</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="16"/>
-        <v>2.5594954089265456</v>
+        <f t="shared" si="2"/>
+        <v>1.0016685200627791</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="16"/>
-        <v>2.2903371231133463</v>
+        <f t="shared" si="2"/>
+        <v>1.0011119346139012</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="16"/>
-        <v>2.049483706521336</v>
-      </c>
-      <c r="G16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.8339585997657344</v>
+        <f t="shared" si="2"/>
+        <v>1.0005557613740521</v>
+      </c>
+      <c r="G16" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.641098260480208</v>
+        <f t="shared" si="2"/>
+        <v>0.99944465014861406</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.4685192462333601</v>
+        <f t="shared" si="2"/>
+        <v>0.99888971147711036</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.3140887590282129</v>
+        <f t="shared" si="2"/>
+        <v>0.99833518364300289</v>
       </c>
       <c r="K16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.1758982873622492</v>
+        <f t="shared" si="2"/>
+        <v>0.99778106630407837</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.0522400201064224</v>
+        <f t="shared" si="2"/>
+        <v>0.99722735911855809</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.9415857407167697</v>
+        <f t="shared" si="2"/>
+        <v>0.9966740617448332</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.84256794094514675</v>
+        <f t="shared" si="2"/>
+        <v>0.99612117384159826</v>
       </c>
       <c r="O16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.75396292064504522</v>
+        <f t="shared" si="2"/>
+        <v>0.99556869506793033</v>
       </c>
       <c r="P16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.67467566481337926</v>
+        <f t="shared" si="2"/>
+        <v>0.99501662508318567</v>
       </c>
       <c r="Q16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.60372631097288498</v>
+        <f t="shared" si="2"/>
+        <v>0.99446496354697733</v>
       </c>
       <c r="R16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.5402380396538361</v>
+        <f t="shared" si="2"/>
+        <v>0.99391371011927065</v>
       </c>
       <c r="S16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.4834262383209732</v>
+        <f t="shared" si="2"/>
+        <v>0.99336286446031929</v>
       </c>
       <c r="T16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.43258880482928042</v>
+        <f t="shared" si="2"/>
+        <v>0.99281242623065635</v>
       </c>
       <c r="U16" s="6">
-        <f t="shared" si="16"/>
-        <v>0.38709747057497801</v>
+        <f t="shared" si="2"/>
+        <v>0.992262395091149</v>
       </c>
       <c r="V16" s="6">
-        <f t="shared" ref="V16:AB16" si="17">EXP(V14 * V12) * (EXP(-V14 * V6) - EXP(-V14 * (V8 + V6))) / (V14 * V8)</f>
-        <v>0.34639003610988384</v>
+        <f t="shared" si="2"/>
+        <v>0.99171277070295005</v>
       </c>
       <c r="W16" s="6">
-        <f t="shared" si="17"/>
-        <v>0.30996342326387333</v>
+        <f t="shared" si="2"/>
+        <v>0.99116355272750589</v>
       </c>
       <c r="X16" s="6">
-        <f t="shared" si="17"/>
-        <v>0.27736745791088774</v>
+        <f t="shared" si="2"/>
+        <v>0.99061474082658374</v>
       </c>
       <c r="Y16" s="6">
-        <f t="shared" si="17"/>
-        <v>0.24819930654351735</v>
+        <f t="shared" si="2"/>
+        <v>0.99006633466223448</v>
       </c>
       <c r="Z16" s="6">
-        <f t="shared" si="17"/>
-        <v>0.22209849790120137</v>
+        <f t="shared" si="2"/>
+        <v>0.98951833389680999</v>
       </c>
       <c r="AA16" s="6">
-        <f t="shared" si="17"/>
-        <v>0.19874246812740876</v>
+        <f t="shared" si="2"/>
+        <v>0.9889707381929731</v>
       </c>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6">
-        <f>2*B7*B5*(B12-B6)*B9*EXP(-B12/B11)*B15</f>
-        <v>-1.337236197540224</v>
+        <f>EXP(B15 * B12) * (EXP(-B15 * B6) - EXP(-B15 * (B8 + B6))) / (B15 * B8)</f>
+        <v>1.0111782702819085</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" ref="C17:U17" si="18">2*C7*C5*(C12-C6)*C9*EXP(-C12/C11)*C15</f>
-        <v>-0.94629172303651632</v>
+        <f t="shared" ref="C17:AA17" si="3">EXP(C15 * C12) * (EXP(-C15 * C6) - EXP(-C15 * (C8 + C6))) / (C15 * C8)</f>
+        <v>1.0100553628234865</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="18"/>
-        <v>-0.62842813157241795</v>
+        <f t="shared" si="3"/>
+        <v>1.0089337023471223</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="18"/>
-        <v>-0.37134532517157826</v>
+        <f t="shared" si="3"/>
+        <v>1.0078132874680497</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="18"/>
-        <v>-0.16474309697157408</v>
-      </c>
-      <c r="G17" s="6" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="3"/>
+        <v>1.0066941168030399</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0055761889704011</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.13009645818687179</v>
+        <f t="shared" si="3"/>
+        <v>1.0044595025899754</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.23157648392212382</v>
+        <f t="shared" si="3"/>
+        <v>1.0033440562831371</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.30947841216999944</v>
+        <f t="shared" si="3"/>
+        <v>1.0022298486727919</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.36800865332861948</v>
+        <f t="shared" si="3"/>
+        <v>1.001116878383375</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.41067603525134655</v>
+        <f t="shared" si="3"/>
+        <v>1.0000051440408486</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.44040462813087888</v>
+        <f t="shared" si="3"/>
+        <v>0.99889464427270114</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.45962848800173517</v>
+        <f t="shared" si="3"/>
+        <v>0.99778537770794506</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.47037120664903925</v>
+        <f t="shared" si="3"/>
+        <v>0.9966773429771153</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.47431269510044394</v>
+        <f t="shared" si="3"/>
+        <v>0.99557053871226764</v>
       </c>
       <c r="Q17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.47284524069961731</v>
+        <f t="shared" si="3"/>
+        <v>0.99446496354697733</v>
       </c>
       <c r="R17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.46712055230918365</v>
+        <f t="shared" si="3"/>
+        <v>0.99336061611633564</v>
       </c>
       <c r="S17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.4580892346291629</v>
+        <f t="shared" si="3"/>
+        <v>0.9922574950569516</v>
       </c>
       <c r="T17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.44653390267275361</v>
+        <f t="shared" si="3"/>
+        <v>0.99115559900694639</v>
       </c>
       <c r="U17" s="6">
-        <f t="shared" si="18"/>
-        <v>0.43309695416203597</v>
+        <f t="shared" si="3"/>
+        <v>0.99005492660595495</v>
       </c>
       <c r="V17" s="6">
-        <f t="shared" ref="V17:AB17" si="19">2*V7*V5*(V12-V6)*V9*EXP(-V12/V11)*V15</f>
-        <v>0.4183038551472632</v>
+        <f t="shared" si="3"/>
+        <v>0.98895547649512205</v>
       </c>
       <c r="W17" s="6">
-        <f t="shared" si="19"/>
-        <v>0.40258265760184903</v>
+        <f t="shared" si="3"/>
+        <v>0.98785724731710189</v>
       </c>
       <c r="X17" s="6">
-        <f t="shared" si="19"/>
-        <v>0.38628035297099012</v>
+        <f t="shared" si="3"/>
+        <v>0.98676023771605559</v>
       </c>
       <c r="Y17" s="6">
-        <f t="shared" si="19"/>
-        <v>0.36967656918344777</v>
+        <f t="shared" si="3"/>
+        <v>0.98566444633765038</v>
       </c>
       <c r="Z17" s="6">
-        <f t="shared" si="19"/>
-        <v>0.35299503755499734</v>
+        <f t="shared" si="3"/>
+        <v>0.98456987182905731</v>
       </c>
       <c r="AA17" s="6">
-        <f t="shared" si="19"/>
-        <v>0.33641318786532087</v>
+        <f t="shared" si="3"/>
+        <v>0.98347651283894932</v>
       </c>
       <c r="AB17" s="6"/>
     </row>
-    <row r="18" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B18" s="6">
-        <f>2*B7*B5*B8*B9*EXP(-B12/B11)*B16</f>
-        <v>6.3928458933058296</v>
+        <f>2*B7*B13*(B12-B6)*B9*EXP(-B12/B11)*B16</f>
+        <v>-1.0027829289631543E-2</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" ref="C18:U18" si="20">2*C7*C5*C8*C9*EXP(-C12/C11)*C16</f>
-        <v>5.3739780453913655</v>
+        <f t="shared" ref="C18:AA18" si="4">2*C7*C13*(C12-C6)*C9*EXP(-C12/C11)*C16</f>
+        <v>-7.5320299484386436E-3</v>
       </c>
       <c r="D18" s="6">
-        <f t="shared" si="20"/>
-        <v>4.5174935411143382</v>
+        <f t="shared" si="4"/>
+        <v>-5.303816198231389E-3</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="20"/>
-        <v>3.7975123310209851</v>
+        <f t="shared" si="4"/>
+        <v>-3.3198037774113489E-3</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="20"/>
-        <v>3.1922790310618039</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="20"/>
-        <v>2.6835055488594204</v>
+        <f t="shared" si="4"/>
+        <v>-1.5584672209294347E-3</v>
+      </c>
+      <c r="G18" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="20"/>
-        <v>2.2558184797411225</v>
+        <f t="shared" si="4"/>
+        <v>1.3738151855842728E-3</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="20"/>
-        <v>1.8962945747231355</v>
+        <f t="shared" si="4"/>
+        <v>2.5797266811167139E-3</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="20"/>
-        <v>1.5940702438686754</v>
+        <f t="shared" si="4"/>
+        <v>3.6331253852959419E-3</v>
       </c>
       <c r="K18" s="6">
-        <f t="shared" si="20"/>
-        <v>1.340013295539034</v>
+        <f t="shared" si="4"/>
+        <v>4.5481481153741609E-3</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="20"/>
-        <v>1.1264469926140295</v>
+        <f t="shared" si="4"/>
+        <v>5.3377734080001958E-3</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.94691808759910112</v>
+        <f t="shared" si="4"/>
+        <v>6.0139102942783386E-3</v>
       </c>
       <c r="N18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.79600182742870773</v>
+        <f t="shared" si="4"/>
+        <v>6.5874805499984432E-3</v>
       </c>
       <c r="O18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.66913803587422704</v>
+        <f t="shared" si="4"/>
+        <v>7.0684948869971995E-3</v>
       </c>
       <c r="P18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.5624933205240914</v>
+        <f t="shared" si="4"/>
+        <v>7.4661235190256591E-3</v>
       </c>
       <c r="Q18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.47284524069961731</v>
+        <f t="shared" si="4"/>
+        <v>7.7887615051586822E-3</v>
       </c>
       <c r="R18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.39748493625481746</v>
+        <f t="shared" si="4"/>
+        <v>8.0440892455288689E-3</v>
       </c>
       <c r="S18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.33413527503360196</v>
+        <f t="shared" si="4"/>
+        <v>8.2391284778606626E-3</v>
       </c>
       <c r="T18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.28088204567885094</v>
+        <f t="shared" si="4"/>
+        <v>8.3802940987951179E-3</v>
       </c>
       <c r="U18" s="6">
-        <f t="shared" si="20"/>
-        <v>0.23611611667400922</v>
+        <f t="shared" si="4"/>
+        <v>8.4734421111974378E-3</v>
       </c>
       <c r="V18" s="6">
-        <f t="shared" ref="V18:AB18" si="21">2*V7*V5*V8*V9*EXP(-V12/V11)*V16</f>
-        <v>0.19848481386011235</v>
+        <f t="shared" si="4"/>
+        <v>8.52391397741715E-3</v>
       </c>
       <c r="W18" s="6">
-        <f t="shared" si="21"/>
-        <v>0.16685104722214014</v>
+        <f t="shared" si="4"/>
+        <v>8.5365776387217318E-3</v>
       </c>
       <c r="X18" s="6">
-        <f t="shared" si="21"/>
-        <v>0.14025895189515777</v>
+        <f t="shared" si="4"/>
+        <v>8.5158654427397815E-3</v>
       </c>
       <c r="Y18" s="6">
-        <f t="shared" si="21"/>
-        <v>0.11790500517828191</v>
+        <f t="shared" si="4"/>
+        <v>8.4658092036412301E-3</v>
       </c>
       <c r="Z18" s="6">
-        <f t="shared" si="21"/>
-        <v>9.9113746810841549E-2</v>
+        <f t="shared" si="4"/>
+        <v>8.3900726038637023E-3</v>
       </c>
       <c r="AA18" s="6">
-        <f t="shared" si="21"/>
-        <v>8.3317368860037988E-2</v>
+        <f t="shared" si="4"/>
+        <v>8.2919811313789706E-3</v>
       </c>
       <c r="AB18" s="6"/>
     </row>
-    <row r="19" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <f>2*B7*B13*B8*B9*EXP(-B12/B11)*B17</f>
+        <v>2.0223565405638171E-2</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" ref="C19:AA19" si="5">2*C7*C13*C8*C9*EXP(-C12/C11)*C17</f>
+        <v>1.897718404002376E-2</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.7807617344690871E-2</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.671013122000255E-2</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.5680283329591677E-2</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.4713905118946942E-2</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.3807084942196058E-2</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.2956152228787828E-2</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.2157662625984023E-2</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.1408384057021666E-2</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.0705283638512867E-2</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.004551540412728E-2</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="5"/>
+        <v>9.4264087848658674E-3</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="5"/>
+        <v>8.8454577992970566E-3</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="5"/>
+        <v>8.300310910000332E-3</v>
+      </c>
+      <c r="Q19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.7887615051586822E-3</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.3087389667719441E-3</v>
+      </c>
+      <c r="S19" s="6">
+        <f t="shared" si="5"/>
+        <v>6.85830028933751E-3</v>
+      </c>
+      <c r="T19" s="6">
+        <f t="shared" si="5"/>
+        <v>6.4356222150729649E-3</v>
+      </c>
+      <c r="U19" s="6">
+        <f t="shared" si="5"/>
+        <v>6.0389938538461755E-3</v>
+      </c>
+      <c r="V19" s="6">
+        <f t="shared" si="5"/>
+        <v>5.6668097579401491E-3</v>
+      </c>
+      <c r="W19" s="6">
+        <f t="shared" si="5"/>
+        <v>5.3175634236212067E-3</v>
+      </c>
+      <c r="X19" s="6">
+        <f t="shared" si="5"/>
+        <v>4.9898411932064613E-3</v>
+      </c>
+      <c r="Y19" s="6">
+        <f t="shared" si="5"/>
+        <v>4.6823165329478002E-3</v>
+      </c>
+      <c r="Z19" s="6">
+        <f t="shared" si="5"/>
+        <v>4.3937446635707329E-3</v>
+      </c>
+      <c r="AA19" s="6">
+        <f t="shared" si="5"/>
+        <v>4.1229575217339321E-3</v>
+      </c>
+      <c r="AB19" s="6"/>
+    </row>
+    <row r="20" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4">
-        <f>IF(B12&lt;=B6,0,IF(B12&lt;B8+B6,B17,B18))</f>
+      <c r="B20" s="8">
+        <f>IF(B12&lt;=B6,0,IF(B12&lt;B8+B6,B18,B19))</f>
         <v>0</v>
       </c>
-      <c r="C19" s="4">
-        <f t="shared" ref="C19:U19" si="22">IF(C12&lt;=C6,0,IF(C12&lt;C8+C6,C17,C18))</f>
+      <c r="C20" s="8">
+        <f t="shared" ref="C20:U20" si="6">IF(C12&lt;=C6,0,IF(C12&lt;C8+C6,C18,C19))</f>
         <v>0</v>
       </c>
-      <c r="D19" s="4">
-        <f t="shared" si="22"/>
+      <c r="D20" s="8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E19" s="4">
-        <f t="shared" si="22"/>
+      <c r="E20" s="8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F19" s="4">
-        <f t="shared" si="22"/>
+      <c r="F20" s="8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G19" s="4">
-        <f t="shared" si="22"/>
+      <c r="G20" s="8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.13009645818687179</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.23157648392212382</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.30947841216999944</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.36800865332861948</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.41067603525134655</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.44040462813087888</v>
-      </c>
-      <c r="N19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.45962848800173517</v>
-      </c>
-      <c r="O19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.47037120664903925</v>
-      </c>
-      <c r="P19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.47431269510044394</v>
-      </c>
-      <c r="Q19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.47284524069961731</v>
-      </c>
-      <c r="R19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.39748493625481746</v>
-      </c>
-      <c r="S19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.33413527503360196</v>
-      </c>
-      <c r="T19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.28088204567885094</v>
-      </c>
-      <c r="U19" s="4">
-        <f t="shared" si="22"/>
-        <v>0.23611611667400922</v>
-      </c>
-      <c r="V19" s="4">
-        <f t="shared" ref="V19" si="23">IF(V12&lt;=V6,0,IF(V12&lt;V8+V6,V17,V18))</f>
-        <v>0.19848481386011235</v>
-      </c>
-      <c r="W19" s="4">
-        <f t="shared" ref="W19" si="24">IF(W12&lt;=W6,0,IF(W12&lt;W8+W6,W17,W18))</f>
-        <v>0.16685104722214014</v>
-      </c>
-      <c r="X19" s="4">
-        <f t="shared" ref="X19" si="25">IF(X12&lt;=X6,0,IF(X12&lt;X8+X6,X17,X18))</f>
-        <v>0.14025895189515777</v>
-      </c>
-      <c r="Y19" s="4">
-        <f t="shared" ref="Y19" si="26">IF(Y12&lt;=Y6,0,IF(Y12&lt;Y8+Y6,Y17,Y18))</f>
-        <v>0.11790500517828191</v>
-      </c>
-      <c r="Z19" s="4">
-        <f t="shared" ref="Z19" si="27">IF(Z12&lt;=Z6,0,IF(Z12&lt;Z8+Z6,Z17,Z18))</f>
-        <v>9.9113746810841549E-2</v>
-      </c>
-      <c r="AA19" s="4">
-        <f t="shared" ref="AA19" si="28">IF(AA12&lt;=AA6,0,IF(AA12&lt;AA8+AA6,AA17,AA18))</f>
-        <v>8.3317368860037988E-2</v>
+      <c r="H20" s="8">
+        <f t="shared" si="6"/>
+        <v>1.3738151855842728E-3</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" si="6"/>
+        <v>2.5797266811167139E-3</v>
+      </c>
+      <c r="J20" s="8">
+        <f t="shared" si="6"/>
+        <v>3.6331253852959419E-3</v>
+      </c>
+      <c r="K20" s="8">
+        <f t="shared" si="6"/>
+        <v>4.5481481153741609E-3</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="6"/>
+        <v>5.3377734080001958E-3</v>
+      </c>
+      <c r="M20" s="8">
+        <f t="shared" si="6"/>
+        <v>6.0139102942783386E-3</v>
+      </c>
+      <c r="N20" s="8">
+        <f t="shared" si="6"/>
+        <v>6.5874805499984432E-3</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="6"/>
+        <v>7.0684948869971995E-3</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="6"/>
+        <v>7.4661235190256591E-3</v>
+      </c>
+      <c r="Q20" s="8">
+        <f t="shared" si="6"/>
+        <v>7.7887615051586822E-3</v>
+      </c>
+      <c r="R20" s="8">
+        <f t="shared" si="6"/>
+        <v>7.3087389667719441E-3</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" si="6"/>
+        <v>6.85830028933751E-3</v>
+      </c>
+      <c r="T20" s="8">
+        <f t="shared" si="6"/>
+        <v>6.4356222150729649E-3</v>
+      </c>
+      <c r="U20" s="8">
+        <f t="shared" si="6"/>
+        <v>6.0389938538461755E-3</v>
+      </c>
+      <c r="V20" s="8">
+        <f t="shared" ref="V20" si="7">IF(V12&lt;=V6,0,IF(V12&lt;V8+V6,V18,V19))</f>
+        <v>5.6668097579401491E-3</v>
+      </c>
+      <c r="W20" s="8">
+        <f t="shared" ref="W20" si="8">IF(W12&lt;=W6,0,IF(W12&lt;W8+W6,W18,W19))</f>
+        <v>5.3175634236212067E-3</v>
+      </c>
+      <c r="X20" s="8">
+        <f t="shared" ref="X20" si="9">IF(X12&lt;=X6,0,IF(X12&lt;X8+X6,X18,X19))</f>
+        <v>4.9898411932064613E-3</v>
+      </c>
+      <c r="Y20" s="8">
+        <f t="shared" ref="Y20" si="10">IF(Y12&lt;=Y6,0,IF(Y12&lt;Y8+Y6,Y18,Y19))</f>
+        <v>4.6823165329478002E-3</v>
+      </c>
+      <c r="Z20" s="8">
+        <f t="shared" ref="Z20" si="11">IF(Z12&lt;=Z6,0,IF(Z12&lt;Z8+Z6,Z18,Z19))</f>
+        <v>4.3937446635707329E-3</v>
+      </c>
+      <c r="AA20" s="8">
+        <f t="shared" ref="AA20" si="12">IF(AA12&lt;=AA6,0,IF(AA12&lt;AA8+AA6,AA18,AA19))</f>
+        <v>4.1229575217339321E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASLDRO-50: Added GKM CASL/pCASL functionality to GkmFilter, also corrected that t1_prime uses t1_tissue and not t1_arterial_blood'
</commit_message>
<xml_diff>
--- a/src/asldro/data/gkm_validation_calculations.xlsx
+++ b/src/asldro/data/gkm_validation_calculations.xlsx
@@ -5,43 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E6BD5C-A31B-4833-B35F-64367411573E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10F817C-C747-4EC4-93D4-9C2AE1412EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PASL" sheetId="1" r:id="rId1"/>
+    <sheet name="CASL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="alpha">PASL!$B$9</definedName>
-    <definedName name="delta_m">PASL!$B$20</definedName>
-    <definedName name="delta_m_arrived">PASL!$B$19</definedName>
-    <definedName name="delta_m_arriving">PASL!$B$18</definedName>
-    <definedName name="delta_m_not_arrived">PASL!$B$18</definedName>
-    <definedName name="delta_m_not_arriving">PASL!$B$18</definedName>
-    <definedName name="delta_t">PASL!$B$6</definedName>
-    <definedName name="f">PASL!$B$5</definedName>
-    <definedName name="k">PASL!$B$15</definedName>
-    <definedName name="label_duration">PASL!$B$8</definedName>
-    <definedName name="label_efficiency">PASL!$B$9</definedName>
-    <definedName name="lambda">PASL!$B$10</definedName>
-    <definedName name="lambda_blood_brain">PASL!$B$10</definedName>
-    <definedName name="m0">PASL!$B$7</definedName>
-    <definedName name="perfusion_rate">PASL!$B$5</definedName>
-    <definedName name="q_pasl_arrived">PASL!$B$17</definedName>
-    <definedName name="q_pasl_arriving">PASL!$B$16</definedName>
-    <definedName name="signal_time">PASL!$B$12</definedName>
-    <definedName name="t">PASL!$B$12</definedName>
-    <definedName name="t1_arterial_blood">PASL!$B$11</definedName>
-    <definedName name="t1_prime">PASL!$B$14</definedName>
-    <definedName name="t1b">PASL!$B$11</definedName>
-    <definedName name="t1p">PASL!$B$14</definedName>
-    <definedName name="tau">PASL!$B$8</definedName>
-    <definedName name="transit_time">PASL!$B$6</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>General Kinetic Model Valitation Calculator</t>
   </si>
@@ -121,6 +95,18 @@
   <si>
     <t>f</t>
   </si>
+  <si>
+    <t>q_ss_arriving</t>
+  </si>
+  <si>
+    <t>q_ss_arrived</t>
+  </si>
+  <si>
+    <t>Continuous ASL</t>
+  </si>
+  <si>
+    <t>t1_tissue</t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +114,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.00000000000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,7 +180,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,7 +245,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PASL!$B$12:$AA$12</c:f>
+              <c:f>PASL!$B$13:$AA$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -346,7 +332,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PASL!$B$20:$AA$20</c:f>
+              <c:f>PASL!$B$21:$AA$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00000000000000E+00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -369,64 +355,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3738151855842728E-3</c:v>
+                  <c:v>1.3677014253934416E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5797266811167139E-3</c:v>
+                  <c:v>2.5568383551978382E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6331253852959419E-3</c:v>
+                  <c:v>3.5849256811777831E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.5481481153741609E-3</c:v>
+                  <c:v>4.467948579457621E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3377734080001958E-3</c:v>
+                  <c:v>5.2204879757336651E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0139102942783386E-3</c:v>
+                  <c:v>5.8558361149690418E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5874805499984432E-3</c:v>
+                  <c:v>6.3861029956216288E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.0684948869971995E-3</c:v>
+                  <c:v>6.8223143711754128E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4661235190256591E-3</c:v>
+                  <c:v>7.1745019687211569E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.7887615051586822E-3</c:v>
+                  <c:v>7.4517865252520235E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3087389667719441E-3</c:v>
+                  <c:v>6.9303763781691664E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.85830028933751E-3</c:v>
+                  <c:v>6.4454499039021743E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.4356222150729649E-3</c:v>
+                  <c:v>5.9944542975438504E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.0389938538461755E-3</c:v>
+                  <c:v>5.5750153769075547E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.6668097579401491E-3</c:v>
+                  <c:v>5.1849250840882415E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.3175634236212067E-3</c:v>
+                  <c:v>4.822129861553788E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.9898411932064613E-3</c:v>
+                  <c:v>4.4847198415746718E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.6823165329478002E-3</c:v>
+                  <c:v>4.1709187920818099E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.3937446635707329E-3</c:v>
+                  <c:v>3.8790747660243834E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.1229575217339321E-3</c:v>
+                  <c:v>3.6076514050029434E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,6 +421,419 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E370-4CC8-BC0D-C2FD5ADB19AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1028898928"/>
+        <c:axId val="678536480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1028898928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678536480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="678536480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00000000000000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028898928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CASL!$B$13:$AA$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CASL!$B$20:$AA$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000000E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4114204094476408E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7240820956291219E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9448953209693643E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.080286828815647E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1362336758283651E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.1182946970801348E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0316397695054022E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8810770277525722E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.6710781757113652E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.040580202696326E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.6776959886316644E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.0005363743893667E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.3707584038460875E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.7850467284305289E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.2403179783566531E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.7337045307989986E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.26253941382758E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.8243422666319836E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.4168062821248605E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0377860631866172E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF37-40E5-B8EB-8CCA16FD6EE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -665,6 +1064,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1181,7 +1620,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>198664</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>59871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>198664</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00356F6A-8CAC-4F9D-A945-071526B25F3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1198,14 +2194,16 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00356F6A-8CAC-4F9D-A945-071526B25F3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B904C710-528E-423E-B7DB-B8FBCEE7084B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1485,9 +2483,1686 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:AA21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5">
+        <v>60</v>
+      </c>
+      <c r="E5" s="5">
+        <v>60</v>
+      </c>
+      <c r="F5" s="5">
+        <v>60</v>
+      </c>
+      <c r="G5" s="5">
+        <v>60</v>
+      </c>
+      <c r="H5" s="5">
+        <v>60</v>
+      </c>
+      <c r="I5" s="5">
+        <v>60</v>
+      </c>
+      <c r="J5" s="5">
+        <v>60</v>
+      </c>
+      <c r="K5" s="5">
+        <v>60</v>
+      </c>
+      <c r="L5" s="5">
+        <v>60</v>
+      </c>
+      <c r="M5" s="5">
+        <v>60</v>
+      </c>
+      <c r="N5" s="5">
+        <v>60</v>
+      </c>
+      <c r="O5" s="5">
+        <v>60</v>
+      </c>
+      <c r="P5" s="5">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>60</v>
+      </c>
+      <c r="R5" s="5">
+        <v>60</v>
+      </c>
+      <c r="S5" s="5">
+        <v>60</v>
+      </c>
+      <c r="T5" s="5">
+        <v>60</v>
+      </c>
+      <c r="U5" s="5">
+        <v>60</v>
+      </c>
+      <c r="V5" s="5">
+        <v>60</v>
+      </c>
+      <c r="W5" s="5">
+        <v>60</v>
+      </c>
+      <c r="X5" s="5">
+        <v>60</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>60</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>60</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>60</v>
+      </c>
+      <c r="AB5" s="5"/>
+    </row>
+    <row r="6" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="X6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AB6" s="5"/>
+    </row>
+    <row r="7" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5">
+        <v>1</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5">
+        <v>1</v>
+      </c>
+      <c r="X7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="5"/>
+    </row>
+    <row r="8" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>1</v>
+      </c>
+      <c r="R8" s="5">
+        <v>1</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1</v>
+      </c>
+      <c r="T8" s="5">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5">
+        <v>1</v>
+      </c>
+      <c r="V8" s="5">
+        <v>1</v>
+      </c>
+      <c r="W8" s="5">
+        <v>1</v>
+      </c>
+      <c r="X8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>1</v>
+      </c>
+      <c r="R9" s="5">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5">
+        <v>1</v>
+      </c>
+      <c r="T9" s="5">
+        <v>1</v>
+      </c>
+      <c r="U9" s="5">
+        <v>1</v>
+      </c>
+      <c r="V9" s="5">
+        <v>1</v>
+      </c>
+      <c r="W9" s="5">
+        <v>1</v>
+      </c>
+      <c r="X9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="5"/>
+    </row>
+    <row r="10" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="AB10" s="5"/>
+    </row>
+    <row r="11" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="N11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="P11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="T11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="V11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="W11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="X11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="R12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="S12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="T12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="U12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="V12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="W12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="X12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N13" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="P13" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="S13" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="T13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="U13" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="V13" s="5">
+        <v>2</v>
+      </c>
+      <c r="W13" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="X13" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="AB13" s="5"/>
+    </row>
+    <row r="14" spans="1:28" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7">
+        <f>B5/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" ref="C14:AA14" si="0">C5/6000</f>
+        <v>0.01</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="P14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="Q14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="R14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="S14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="T14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="U14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="V14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="X14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="Y14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="Z14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="AA14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="AB14" s="7"/>
+    </row>
+    <row r="15" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6">
+        <f>1/(1/B12+B14/B10)</f>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:AA15" si="1">1/(1/C12+C14/C10)</f>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="Q15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="R15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="S15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="T15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="U15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="V15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="W15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="X15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="Y15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="Z15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="AA15" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3785557986870898</v>
+      </c>
+      <c r="AB15" s="6"/>
+    </row>
+    <row r="16" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6">
+        <f>(1/B11-1/B15)</f>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:AA16" si="2">(1/C11-1/C15)</f>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="P16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="R16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="S16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="T16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="U16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="V16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="W16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="X16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="Y16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="Z16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="AA16" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.10039682539682537</v>
+      </c>
+      <c r="AB16" s="6"/>
+    </row>
+    <row r="17" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6">
+        <f>EXP(B16 * B13) * (EXP(- B16 * B6) - EXP(- B16 * B13)) / (B16 * (B13 - B6))</f>
+        <v>1.0255245104000086</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" ref="C17:AA17" si="3">EXP(C16 * C13) * (EXP(- C16 * C6) - EXP(- C16 * C13)) / (C16 * (C13 - C6))</f>
+        <v>1.0203508727060766</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="3"/>
+        <v>1.015211861986193</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0101072180331994</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0050366827235562</v>
+      </c>
+      <c r="G17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.99499691585426719</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.99002717831006848</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.98509053740615937</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.98018674517953097</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.97531555564879435</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.97047672479767744</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.96567001055865997</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.96089517279677494</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.95615197329352719</v>
+      </c>
+      <c r="Q17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.95144017573094675</v>
+      </c>
+      <c r="R17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.94675954567579967</v>
+      </c>
+      <c r="S17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.94210985056390995</v>
+      </c>
+      <c r="T17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.93749085968463763</v>
+      </c>
+      <c r="U17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.93290234416546902</v>
+      </c>
+      <c r="V17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.92834407695675181</v>
+      </c>
+      <c r="W17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.92381583281656143</v>
+      </c>
+      <c r="X17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.91931738829568377</v>
+      </c>
+      <c r="Y17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.91484852172274478</v>
+      </c>
+      <c r="Z17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.91040901318945089</v>
+      </c>
+      <c r="AA17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.90599864453596235</v>
+      </c>
+      <c r="AB17" s="6"/>
+    </row>
+    <row r="18" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <f>EXP(B16 * B13) * (EXP(-B16 * B6) - EXP(-B16 * (B8 + B6))) / (B16 * B8)</f>
+        <v>1.106073957520527</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:AA18" si="4">EXP(C16 * C13) * (EXP(-C16 * C6) - EXP(-C16 * (C8 + C6))) / (C16 * C8)</f>
+        <v>1.0950248835269067</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0840861837404416</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0732567555831596</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0625355074912379</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0519213588049809</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0414132396598921</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0310100908788358</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0207108638652769</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0105145204975863</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0004200330244029</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.99042638396103866</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.98053256598692173</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.97073758184406189</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.9610404442365309</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.95144017573094675</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.94193580865795279</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.93252638501467988</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.9232109563681834</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.91398858375984571</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.90485833761073209</v>
+      </c>
+      <c r="W18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.89581929762789292</v>
+      </c>
+      <c r="X18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.88687055271160209</v>
+      </c>
+      <c r="Y18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.87801120086352147</v>
+      </c>
+      <c r="Z18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.86924034909578307</v>
+      </c>
+      <c r="AA18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.86055711334097928</v>
+      </c>
+      <c r="AB18" s="6"/>
+    </row>
+    <row r="19" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <f>2*B7*B14*(B13-B6)*B9*EXP(-B13/B11)*B17</f>
+        <v>-1.0255245104000086E-2</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" ref="C19:AA19" si="5">2*C7*C14*(C13-C6)*C9*EXP(-C13/C11)*C17</f>
+        <v>-7.668247507785747E-3</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="5"/>
+        <v>-5.3755279420197302E-3</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="5"/>
+        <v>-3.3496331849348828E-3</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="5"/>
+        <v>-1.565446711041185E-3</v>
+      </c>
+      <c r="G19" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.3677014253934416E-3</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5568383551978382E-3</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="5"/>
+        <v>3.5849256811777831E-3</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="5"/>
+        <v>4.467948579457621E-3</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="5"/>
+        <v>5.2204879757336651E-3</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" si="5"/>
+        <v>5.8558361149690418E-3</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="5"/>
+        <v>6.3861029956216288E-3</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="5"/>
+        <v>6.8223143711754128E-3</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.1745019687211569E-3</v>
+      </c>
+      <c r="Q19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.4517865252520235E-3</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.6624541969127205E-3</v>
+      </c>
+      <c r="S19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.8140268543975041E-3</v>
+      </c>
+      <c r="T19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.9133267387854703E-3</v>
+      </c>
+      <c r="U19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.9665359160974239E-3</v>
+      </c>
+      <c r="V19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.9792509355456447E-3</v>
+      </c>
+      <c r="W19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.9565330656252049E-3</v>
+      </c>
+      <c r="X19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.9029544536804996E-3</v>
+      </c>
+      <c r="Y19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.8226405282027945E-3</v>
+      </c>
+      <c r="Z19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.7193089387143738E-3</v>
+      </c>
+      <c r="AA19" s="6">
+        <f t="shared" si="5"/>
+        <v>7.5963053055278984E-3</v>
+      </c>
+      <c r="AB19" s="6"/>
+    </row>
+    <row r="20" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6">
+        <f>2*B7*B14*B8*B9*EXP(-B13/B11)*B18</f>
+        <v>2.2121479150410541E-2</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" ref="C20:AA20" si="6">2*C7*C14*C8*C9*EXP(-C13/C11)*C18</f>
+        <v>2.0573613593819623E-2</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.9134053985713887E-2</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.7795222033245288E-2</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.6550069705506973E-2</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.5392042130490243E-2</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.4315043088184343E-2</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.3313402918164147E-2</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2381848672721166E-2</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1515476358414578E-2</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="6"/>
+        <v>1.0709725119913147E-2</v>
+      </c>
+      <c r="M20" s="6">
+        <f t="shared" si="6"/>
+        <v>9.9603532302236421E-3</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="6"/>
+        <v>9.2634157609108765E-3</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="6"/>
+        <v>8.6152438147582919E-3</v>
+      </c>
+      <c r="P20" s="6">
+        <f t="shared" si="6"/>
+        <v>8.0124252115434252E-3</v>
+      </c>
+      <c r="Q20" s="6">
+        <f t="shared" si="6"/>
+        <v>7.4517865252520235E-3</v>
+      </c>
+      <c r="R20" s="6">
+        <f t="shared" si="6"/>
+        <v>6.9303763781691664E-3</v>
+      </c>
+      <c r="S20" s="6">
+        <f t="shared" si="6"/>
+        <v>6.4454499039021743E-3</v>
+      </c>
+      <c r="T20" s="6">
+        <f t="shared" si="6"/>
+        <v>5.9944542975438504E-3</v>
+      </c>
+      <c r="U20" s="6">
+        <f t="shared" si="6"/>
+        <v>5.5750153769075547E-3</v>
+      </c>
+      <c r="V20" s="6">
+        <f t="shared" si="6"/>
+        <v>5.1849250840882415E-3</v>
+      </c>
+      <c r="W20" s="6">
+        <f t="shared" si="6"/>
+        <v>4.822129861553788E-3</v>
+      </c>
+      <c r="X20" s="6">
+        <f t="shared" si="6"/>
+        <v>4.4847198415746718E-3</v>
+      </c>
+      <c r="Y20" s="6">
+        <f t="shared" si="6"/>
+        <v>4.1709187920818099E-3</v>
+      </c>
+      <c r="Z20" s="6">
+        <f t="shared" si="6"/>
+        <v>3.8790747660243834E-3</v>
+      </c>
+      <c r="AA20" s="6">
+        <f t="shared" si="6"/>
+        <v>3.6076514050029434E-3</v>
+      </c>
+      <c r="AB20" s="6"/>
+    </row>
+    <row r="21" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="8">
+        <f>IF(B13&lt;=B6,0,IF(B13&lt;B8+B6,B19,B20))</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <f t="shared" ref="C21:U21" si="7">IF(C13&lt;=C6,0,IF(C13&lt;C8+C6,C19,C20))</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="7"/>
+        <v>1.3677014253934416E-3</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="7"/>
+        <v>2.5568383551978382E-3</v>
+      </c>
+      <c r="J21" s="8">
+        <f t="shared" si="7"/>
+        <v>3.5849256811777831E-3</v>
+      </c>
+      <c r="K21" s="8">
+        <f t="shared" si="7"/>
+        <v>4.467948579457621E-3</v>
+      </c>
+      <c r="L21" s="8">
+        <f t="shared" si="7"/>
+        <v>5.2204879757336651E-3</v>
+      </c>
+      <c r="M21" s="8">
+        <f t="shared" si="7"/>
+        <v>5.8558361149690418E-3</v>
+      </c>
+      <c r="N21" s="8">
+        <f t="shared" si="7"/>
+        <v>6.3861029956216288E-3</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" si="7"/>
+        <v>6.8223143711754128E-3</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="7"/>
+        <v>7.1745019687211569E-3</v>
+      </c>
+      <c r="Q21" s="8">
+        <f t="shared" si="7"/>
+        <v>7.4517865252520235E-3</v>
+      </c>
+      <c r="R21" s="8">
+        <f t="shared" si="7"/>
+        <v>6.9303763781691664E-3</v>
+      </c>
+      <c r="S21" s="8">
+        <f t="shared" si="7"/>
+        <v>6.4454499039021743E-3</v>
+      </c>
+      <c r="T21" s="8">
+        <f t="shared" si="7"/>
+        <v>5.9944542975438504E-3</v>
+      </c>
+      <c r="U21" s="8">
+        <f t="shared" si="7"/>
+        <v>5.5750153769075547E-3</v>
+      </c>
+      <c r="V21" s="8">
+        <f t="shared" ref="V21" si="8">IF(V13&lt;=V6,0,IF(V13&lt;V8+V6,V19,V20))</f>
+        <v>5.1849250840882415E-3</v>
+      </c>
+      <c r="W21" s="8">
+        <f t="shared" ref="W21" si="9">IF(W13&lt;=W6,0,IF(W13&lt;W8+W6,W19,W20))</f>
+        <v>4.822129861553788E-3</v>
+      </c>
+      <c r="X21" s="8">
+        <f t="shared" ref="X21" si="10">IF(X13&lt;=X6,0,IF(X13&lt;X8+X6,X19,X20))</f>
+        <v>4.4847198415746718E-3</v>
+      </c>
+      <c r="Y21" s="8">
+        <f t="shared" ref="Y21" si="11">IF(Y13&lt;=Y6,0,IF(Y13&lt;Y8+Y6,Y19,Y20))</f>
+        <v>4.1709187920818099E-3</v>
+      </c>
+      <c r="Z21" s="8">
+        <f t="shared" ref="Z21" si="12">IF(Z13&lt;=Z6,0,IF(Z13&lt;Z8+Z6,Z19,Z20))</f>
+        <v>3.8790747660243834E-3</v>
+      </c>
+      <c r="AA21" s="8">
+        <f t="shared" ref="AA21" si="13">IF(AA13&lt;=AA6,0,IF(AA13&lt;AA8+AA6,AA19,AA20))</f>
+        <v>3.6076514050029434E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="193" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76AA146-4C14-4EFF-9DA6-89F1F35E3AF0}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:AA20"/>
     </sheetView>
   </sheetViews>
@@ -1510,7 +4185,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2106,637 +4781,611 @@
       </c>
       <c r="AB11" s="5"/>
     </row>
-    <row r="12" spans="1:28" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="C12" s="5">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="D12" s="5">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="E12" s="5">
-        <v>0.3</v>
+        <v>1.4</v>
       </c>
       <c r="F12" s="5">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="G12" s="5">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="H12" s="5">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="I12" s="5">
-        <v>0.7</v>
+        <v>1.4</v>
       </c>
       <c r="J12" s="5">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="K12" s="5">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="M12" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="N12" s="5">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="O12" s="5">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="P12" s="5">
         <v>1.4</v>
       </c>
       <c r="Q12" s="5">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="R12" s="5">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="S12" s="5">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="T12" s="5">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="U12" s="5">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="V12" s="5">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="W12" s="5">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="X12" s="5">
-        <v>2.2000000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="Y12" s="5">
-        <v>2.2999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="Z12" s="5">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="AA12" s="5">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
       <c r="AB12" s="5"/>
     </row>
-    <row r="13" spans="1:28" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:28" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N13" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="P13" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="S13" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="T13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="U13" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="V13" s="5">
+        <v>2</v>
+      </c>
+      <c r="W13" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="X13" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="AB13" s="5"/>
+    </row>
+    <row r="14" spans="1:28" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7">
-        <f>f/6000</f>
+      <c r="B14" s="7">
+        <f>B5/6000</f>
         <v>0.01</v>
       </c>
-      <c r="C13" s="7">
-        <f>f/6000</f>
+      <c r="C14" s="7">
+        <f t="shared" ref="C14:AA14" si="0">C5/6000</f>
         <v>0.01</v>
       </c>
-      <c r="D13" s="7">
-        <f>f/6000</f>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="E13" s="7">
-        <f>f/6000</f>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="F13" s="7">
-        <f>f/6000</f>
+      <c r="F14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="G13" s="7">
-        <f>f/6000</f>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="H13" s="7">
-        <f>f/6000</f>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="I13" s="7">
-        <f>f/6000</f>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="J13" s="7">
-        <f>f/6000</f>
+      <c r="J14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="K13" s="7">
-        <f>f/6000</f>
+      <c r="K14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="L13" s="7">
-        <f>f/6000</f>
+      <c r="L14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="M13" s="7">
-        <f>f/6000</f>
+      <c r="M14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="N13" s="7">
-        <f>f/6000</f>
+      <c r="N14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="O13" s="7">
-        <f>f/6000</f>
+      <c r="O14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="P13" s="7">
-        <f>f/6000</f>
+      <c r="P14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="Q13" s="7">
-        <f>f/6000</f>
+      <c r="Q14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="R13" s="7">
-        <f>f/6000</f>
+      <c r="R14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="S13" s="7">
-        <f>f/6000</f>
+      <c r="S14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="T13" s="7">
-        <f>f/6000</f>
+      <c r="T14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="U13" s="7">
-        <f>f/6000</f>
+      <c r="U14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="V13" s="7">
-        <f>f/6000</f>
+      <c r="V14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="W13" s="7">
-        <f>f/6000</f>
+      <c r="W14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="X13" s="7">
-        <f>f/6000</f>
+      <c r="X14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="Y13" s="7">
-        <f>f/6000</f>
+      <c r="Y14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="Z13" s="7">
-        <f>f/6000</f>
+      <c r="Z14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="AA13" s="7">
-        <f>f/6000</f>
+      <c r="AA14" s="7">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="AB13" s="7"/>
-    </row>
-    <row r="14" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6">
-        <f>1/(1/B11+B13/B10)</f>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="C14" s="6">
-        <f t="shared" ref="C14:AA14" si="0">1/(1/C11+C13/C10)</f>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="D14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="E14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="F14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="H14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="I14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="J14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="K14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="L14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="N14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="O14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="P14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="Q14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="R14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="S14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="T14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="U14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="V14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="W14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="X14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="Y14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="Z14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="AA14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.572052401746725</v>
-      </c>
-      <c r="AB14" s="6"/>
+      <c r="AB14" s="7"/>
     </row>
     <row r="15" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6">
-        <f>(1/B11-1/B14)</f>
-        <v>-1.1111111111111072E-2</v>
+        <f>1/(1/B12+B14/B10)</f>
+        <v>1.3785557986870898</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" ref="C15:AA15" si="1">(1/C11-1/C14)</f>
-        <v>-1.1111111111111072E-2</v>
+        <f t="shared" ref="C15:AA15" si="1">1/(1/C12+C14/C10)</f>
+        <v>1.3785557986870898</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="J15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="S15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="T15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="U15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="V15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="W15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="X15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="Y15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="Z15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="AA15" s="6">
         <f t="shared" si="1"/>
-        <v>-1.1111111111111072E-2</v>
+        <v>1.3785557986870898</v>
       </c>
       <c r="AB15" s="6"/>
     </row>
     <row r="16" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6">
-        <f>EXP(B15 * B12) * (EXP(- B15 * B6) - EXP(- B15 * B12)) / (B15 * (B12 - B6))</f>
-        <v>1.0027829289631542</v>
+        <f>1-EXP(-(B13-B6)/B15)</f>
+        <v>-0.43720235189519707</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" ref="C16:AA16" si="2">EXP(C15 * C12) * (EXP(- C15 * C6) - EXP(- C15 * C12)) / (C15 * (C12 - C6))</f>
-        <v>1.0022255180645383</v>
+        <f t="shared" ref="C16:AA16" si="2">1-EXP(-(C13-C6)/C15)</f>
+        <v>-0.33663963620948989</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="2"/>
-        <v>1.0016685200627791</v>
+        <v>-0.24311341039088363</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="2"/>
-        <v>1.0011119346139012</v>
+        <v>-0.15613132308120159</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" si="2"/>
-        <v>1.0005557613740521</v>
-      </c>
-      <c r="G16" s="6" t="e">
+        <v>-7.5235473317915469E-2</v>
+      </c>
+      <c r="G16" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99944465014861406</v>
+        <v>6.9971159978341357E-2</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99888971147711036</v>
+        <v>0.13504635672796794</v>
       </c>
       <c r="J16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99833518364300289</v>
+        <v>0.19556816647520459</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99778106630407837</v>
+        <v>0.25185519499043851</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99722735911855809</v>
+        <v>0.30420375482872741</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" si="2"/>
-        <v>0.9966740617448332</v>
+        <v>0.35288942521193578</v>
       </c>
       <c r="N16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99612117384159826</v>
+        <v>0.39816850276410787</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99556869506793033</v>
+        <v>0.44027935073720514</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99501662508318567</v>
+        <v>0.47944365382995324</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99446496354697733</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99391371011927065</v>
+        <v>0.549742891851841</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99336286446031929</v>
+        <v>0.58124790399746118</v>
       </c>
       <c r="T16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99281242623065635</v>
+        <v>0.6105484738981205</v>
       </c>
       <c r="U16" s="6">
         <f t="shared" si="2"/>
-        <v>0.992262395091149</v>
+        <v>0.63779884893480432</v>
       </c>
       <c r="V16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99171277070295005</v>
+        <v>0.66314248362032646</v>
       </c>
       <c r="W16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99116355272750589</v>
+        <v>0.6867127947888354</v>
       </c>
       <c r="X16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99061474082658374</v>
+        <v>0.70863386394383321</v>
       </c>
       <c r="Y16" s="6">
         <f t="shared" si="2"/>
-        <v>0.99006633466223448</v>
+        <v>0.7290210904620904</v>
       </c>
       <c r="Z16" s="6">
         <f t="shared" si="2"/>
-        <v>0.98951833389680999</v>
+        <v>0.74798179909212392</v>
       </c>
       <c r="AA16" s="6">
         <f t="shared" si="2"/>
-        <v>0.9889707381929731</v>
+        <v>0.76561580494530279</v>
       </c>
       <c r="AB16" s="6"/>
     </row>
     <row r="17" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B17" s="6">
-        <f>EXP(B15 * B12) * (EXP(-B15 * B6) - EXP(-B15 * (B8 + B6))) / (B15 * B8)</f>
-        <v>1.0111782702819085</v>
+        <f>1-EXP(-B8/B15)</f>
+        <v>0.51586758520555842</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" ref="C17:AA17" si="3">EXP(C15 * C12) * (EXP(-C15 * C6) - EXP(-C15 * (C8 + C6))) / (C15 * C8)</f>
-        <v>1.0100553628234865</v>
+        <f t="shared" ref="C17:AA17" si="3">1-EXP(-C8/C15)</f>
+        <v>0.51586758520555842</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0089337023471223</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0078132874680497</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0066941168030399</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0055761889704011</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0044595025899754</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0033440562831371</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0022298486727919</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" si="3"/>
-        <v>1.001116878383375</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="3"/>
-        <v>1.0000051440408486</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99889464427270114</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="N17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99778537770794506</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
-        <v>0.9966773429771153</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99557053871226764</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99446496354697733</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99336061611633564</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" si="3"/>
-        <v>0.9922574950569516</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="T17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99115559900694639</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="U17" s="6">
         <f t="shared" si="3"/>
-        <v>0.99005492660595495</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="V17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98895547649512205</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="W17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98785724731710189</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="X17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98676023771605559</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="Y17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98566444633765038</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="Z17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98456987182905731</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="AA17" s="6">
         <f t="shared" si="3"/>
-        <v>0.98347651283894932</v>
+        <v>0.51586758520555842</v>
       </c>
       <c r="AB17" s="6"/>
     </row>
@@ -2745,108 +5394,108 @@
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <f>2*B7*B13*(B12-B6)*B9*EXP(-B12/B11)*B16</f>
-        <v>-1.0027829289631543E-2</v>
+        <f>2*B7*B14*B15*B9*EXP(-B6/B11)*B16</f>
+        <v>-8.8190094706790401E-3</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" ref="C18:AA18" si="4">2*C7*C13*(C12-C6)*C9*EXP(-C12/C11)*C16</f>
-        <v>-7.5320299484386436E-3</v>
+        <f t="shared" ref="C18:AA18" si="4">2*C7*C14*C15*C9*EXP(-C6/C11)*C16</f>
+        <v>-6.79051273870801E-3</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="4"/>
-        <v>-5.303816198231389E-3</v>
+        <v>-4.9039522760852654E-3</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="4"/>
-        <v>-3.3198037774113489E-3</v>
+        <v>-3.149396637401511E-3</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" si="4"/>
-        <v>-1.5584672209294347E-3</v>
-      </c>
-      <c r="G18" s="6" t="e">
+        <v>-1.5176092920030004E-3</v>
+      </c>
+      <c r="G18" s="6">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="4"/>
-        <v>1.3738151855842728E-3</v>
+        <v>1.4114204094476408E-3</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="4"/>
-        <v>2.5797266811167139E-3</v>
+        <v>2.7240820956291219E-3</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="4"/>
-        <v>3.6331253852959419E-3</v>
+        <v>3.9448953209693643E-3</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" si="4"/>
-        <v>4.5481481153741609E-3</v>
+        <v>5.080286828815647E-3</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="4"/>
-        <v>5.3377734080001958E-3</v>
+        <v>6.1362336758283651E-3</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" si="4"/>
-        <v>6.0139102942783386E-3</v>
+        <v>7.1182946970801348E-3</v>
       </c>
       <c r="N18" s="6">
         <f t="shared" si="4"/>
-        <v>6.5874805499984432E-3</v>
+        <v>8.0316397695054022E-3</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="4"/>
-        <v>7.0684948869971995E-3</v>
+        <v>8.8810770277525722E-3</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="4"/>
-        <v>7.4661235190256591E-3</v>
+        <v>9.6710781757113652E-3</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="4"/>
-        <v>7.7887615051586822E-3</v>
+        <v>1.040580202696326E-2</v>
       </c>
       <c r="R18" s="6">
         <f t="shared" si="4"/>
-        <v>8.0440892455288689E-3</v>
+        <v>1.1089116398079305E-2</v>
       </c>
       <c r="S18" s="6">
         <f t="shared" si="4"/>
-        <v>8.2391284778606626E-3</v>
+        <v>1.172461847001849E-2</v>
       </c>
       <c r="T18" s="6">
         <f t="shared" si="4"/>
-        <v>8.3802940987951179E-3</v>
+        <v>1.231565372481545E-2</v>
       </c>
       <c r="U18" s="6">
         <f t="shared" si="4"/>
-        <v>8.4734421111974378E-3</v>
+        <v>1.2865333557246174E-2</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="4"/>
-        <v>8.52391397741715E-3</v>
+        <v>1.3376551654185017E-2</v>
       </c>
       <c r="W18" s="6">
         <f t="shared" si="4"/>
-        <v>8.5365776387217318E-3</v>
+        <v>1.3851999227879134E-2</v>
       </c>
       <c r="X18" s="6">
         <f t="shared" si="4"/>
-        <v>8.5158654427397815E-3</v>
+        <v>1.4294179183332981E-2</v>
       </c>
       <c r="Y18" s="6">
         <f t="shared" si="4"/>
-        <v>8.4658092036412301E-3</v>
+        <v>1.4705419294384552E-2</v>
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="4"/>
-        <v>8.3900726038637023E-3</v>
+        <v>1.5087884457836223E-2</v>
       </c>
       <c r="AA18" s="6">
         <f t="shared" si="4"/>
-        <v>8.2919811313789706E-3</v>
+        <v>1.5443588090149878E-2</v>
       </c>
       <c r="AB18" s="6"/>
     </row>
@@ -2855,108 +5504,108 @@
         <v>14</v>
       </c>
       <c r="B19" s="6">
-        <f>2*B7*B13*B8*B9*EXP(-B12/B11)*B17</f>
-        <v>2.0223565405638171E-2</v>
+        <f>2*B7*B14*B15*B9*EXP(-B6/B11)*EXP(-(B13-B8-B6)/B15)*B17</f>
+        <v>3.0890811458797421E-2</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" ref="C19:AA19" si="5">2*C7*C13*C8*C9*EXP(-C12/C11)*C17</f>
-        <v>1.897718404002376E-2</v>
+        <f t="shared" ref="C19:AA19" si="5">2*C7*C14*C15*C9*EXP(-C6/C11)*EXP(-(C13-C8-C6)/C15)*C17</f>
+        <v>2.8729345548353134E-2</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="5"/>
-        <v>1.7807617344690871E-2</v>
+        <v>2.6719119914916267E-2</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="5"/>
-        <v>1.671013122000255E-2</v>
+        <v>2.4849552100869175E-2</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" si="5"/>
-        <v>1.5680283329591677E-2</v>
+        <v>2.3110800115429132E-2</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="5"/>
-        <v>1.4713905118946942E-2</v>
+        <v>2.1493710623324964E-2</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="5"/>
-        <v>1.3807084942196058E-2</v>
+        <v>1.9989770758772122E-2</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="5"/>
-        <v>1.2956152228787828E-2</v>
+        <v>1.8591063311079709E-2</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" si="5"/>
-        <v>1.2157662625984023E-2</v>
+        <v>1.729022504597268E-2</v>
       </c>
       <c r="K19" s="6">
         <f t="shared" si="5"/>
-        <v>1.1408384057021666E-2</v>
+        <v>1.60804079432194E-2</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="5"/>
-        <v>1.0705283638512867E-2</v>
+        <v>1.4955243146507405E-2</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="5"/>
-        <v>1.004551540412728E-2</v>
+        <v>1.3908807435788142E-2</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="5"/>
-        <v>9.4264087848658674E-3</v>
+        <v>1.2935592045590668E-2</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="5"/>
-        <v>8.8454577992970566E-3</v>
+        <v>1.2030473665154083E-2</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="5"/>
-        <v>8.300310910000332E-3</v>
+        <v>1.1188687467714365E-2</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="5"/>
-        <v>7.7887615051586822E-3</v>
+        <v>1.040580202696326E-2</v>
       </c>
       <c r="R19" s="6">
         <f t="shared" si="5"/>
-        <v>7.3087389667719441E-3</v>
+        <v>9.6776959886316644E-3</v>
       </c>
       <c r="S19" s="6">
         <f t="shared" si="5"/>
-        <v>6.85830028933751E-3</v>
+        <v>9.0005363743893667E-3</v>
       </c>
       <c r="T19" s="6">
         <f t="shared" si="5"/>
-        <v>6.4356222150729649E-3</v>
+        <v>8.3707584038460875E-3</v>
       </c>
       <c r="U19" s="6">
         <f t="shared" si="5"/>
-        <v>6.0389938538461755E-3</v>
+        <v>7.7850467284305289E-3</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="5"/>
-        <v>5.6668097579401491E-3</v>
+        <v>7.2403179783566531E-3</v>
       </c>
       <c r="W19" s="6">
         <f t="shared" si="5"/>
-        <v>5.3175634236212067E-3</v>
+        <v>6.7337045307989986E-3</v>
       </c>
       <c r="X19" s="6">
         <f t="shared" si="5"/>
-        <v>4.9898411932064613E-3</v>
+        <v>6.26253941382758E-3</v>
       </c>
       <c r="Y19" s="6">
         <f t="shared" si="5"/>
-        <v>4.6823165329478002E-3</v>
+        <v>5.8243422666319836E-3</v>
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="5"/>
-        <v>4.3937446635707329E-3</v>
+        <v>5.4168062821248605E-3</v>
       </c>
       <c r="AA19" s="6">
         <f t="shared" si="5"/>
-        <v>4.1229575217339321E-3</v>
+        <v>5.0377860631866172E-3</v>
       </c>
       <c r="AB19" s="6"/>
     </row>
@@ -2965,11 +5614,11 @@
         <v>15</v>
       </c>
       <c r="B20" s="8">
-        <f>IF(B12&lt;=B6,0,IF(B12&lt;B8+B6,B18,B19))</f>
+        <f>IF(B13&lt;=B6,0,IF(B13&lt;B8+B6,B18,B19))</f>
         <v>0</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" ref="C20:U20" si="6">IF(C12&lt;=C6,0,IF(C12&lt;C8+C6,C18,C19))</f>
+        <f t="shared" ref="C20:AA20" si="6">IF(C13&lt;=C6,0,IF(C13&lt;C8+C6,C18,C19))</f>
         <v>0</v>
       </c>
       <c r="D20" s="8">
@@ -2990,83 +5639,83 @@
       </c>
       <c r="H20" s="8">
         <f t="shared" si="6"/>
-        <v>1.3738151855842728E-3</v>
+        <v>1.4114204094476408E-3</v>
       </c>
       <c r="I20" s="8">
         <f t="shared" si="6"/>
-        <v>2.5797266811167139E-3</v>
+        <v>2.7240820956291219E-3</v>
       </c>
       <c r="J20" s="8">
         <f t="shared" si="6"/>
-        <v>3.6331253852959419E-3</v>
+        <v>3.9448953209693643E-3</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="6"/>
-        <v>4.5481481153741609E-3</v>
+        <v>5.080286828815647E-3</v>
       </c>
       <c r="L20" s="8">
         <f t="shared" si="6"/>
-        <v>5.3377734080001958E-3</v>
+        <v>6.1362336758283651E-3</v>
       </c>
       <c r="M20" s="8">
         <f t="shared" si="6"/>
-        <v>6.0139102942783386E-3</v>
+        <v>7.1182946970801348E-3</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="6"/>
-        <v>6.5874805499984432E-3</v>
+        <v>8.0316397695054022E-3</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" si="6"/>
-        <v>7.0684948869971995E-3</v>
+        <v>8.8810770277525722E-3</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="6"/>
-        <v>7.4661235190256591E-3</v>
+        <v>9.6710781757113652E-3</v>
       </c>
       <c r="Q20" s="8">
         <f t="shared" si="6"/>
-        <v>7.7887615051586822E-3</v>
+        <v>1.040580202696326E-2</v>
       </c>
       <c r="R20" s="8">
         <f t="shared" si="6"/>
-        <v>7.3087389667719441E-3</v>
+        <v>9.6776959886316644E-3</v>
       </c>
       <c r="S20" s="8">
         <f t="shared" si="6"/>
-        <v>6.85830028933751E-3</v>
+        <v>9.0005363743893667E-3</v>
       </c>
       <c r="T20" s="8">
         <f t="shared" si="6"/>
-        <v>6.4356222150729649E-3</v>
+        <v>8.3707584038460875E-3</v>
       </c>
       <c r="U20" s="8">
         <f t="shared" si="6"/>
-        <v>6.0389938538461755E-3</v>
+        <v>7.7850467284305289E-3</v>
       </c>
       <c r="V20" s="8">
-        <f t="shared" ref="V20" si="7">IF(V12&lt;=V6,0,IF(V12&lt;V8+V6,V18,V19))</f>
-        <v>5.6668097579401491E-3</v>
+        <f t="shared" si="6"/>
+        <v>7.2403179783566531E-3</v>
       </c>
       <c r="W20" s="8">
-        <f t="shared" ref="W20" si="8">IF(W12&lt;=W6,0,IF(W12&lt;W8+W6,W18,W19))</f>
-        <v>5.3175634236212067E-3</v>
+        <f t="shared" si="6"/>
+        <v>6.7337045307989986E-3</v>
       </c>
       <c r="X20" s="8">
-        <f t="shared" ref="X20" si="9">IF(X12&lt;=X6,0,IF(X12&lt;X8+X6,X18,X19))</f>
-        <v>4.9898411932064613E-3</v>
+        <f t="shared" si="6"/>
+        <v>6.26253941382758E-3</v>
       </c>
       <c r="Y20" s="8">
-        <f t="shared" ref="Y20" si="10">IF(Y12&lt;=Y6,0,IF(Y12&lt;Y8+Y6,Y18,Y19))</f>
-        <v>4.6823165329478002E-3</v>
+        <f t="shared" si="6"/>
+        <v>5.8243422666319836E-3</v>
       </c>
       <c r="Z20" s="8">
-        <f t="shared" ref="Z20" si="11">IF(Z12&lt;=Z6,0,IF(Z12&lt;Z8+Z6,Z18,Z19))</f>
-        <v>4.3937446635707329E-3</v>
+        <f t="shared" si="6"/>
+        <v>5.4168062821248605E-3</v>
       </c>
       <c r="AA20" s="8">
-        <f t="shared" ref="AA20" si="12">IF(AA12&lt;=AA6,0,IF(AA12&lt;AA8+AA6,AA18,AA19))</f>
-        <v>4.1229575217339321E-3</v>
+        <f t="shared" si="6"/>
+        <v>5.0377860631866172E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>